<commit_message>
New experiments on big dataset.
</commit_message>
<xml_diff>
--- a/docs/benchmarks/finance_queries.xlsx
+++ b/docs/benchmarks/finance_queries.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17240" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="finance.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="standard" sheetId="1" r:id="rId1"/>
+    <sheet name="big" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="18">
   <si>
     <t>Dataset</t>
   </si>
@@ -177,7 +178,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>finance.csv!$C$1</c:f>
+              <c:f>standard!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -189,7 +190,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>finance.csv!$A$3:$A$7</c:f>
+              <c:f>standard!$A$3:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -212,7 +213,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>finance.csv!$G$10:$G$14</c:f>
+              <c:f>standard!$G$10:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -240,7 +241,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>finance.csv!$H$1</c:f>
+              <c:f>standard!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -252,7 +253,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>finance.csv!$A$3:$A$7</c:f>
+              <c:f>standard!$A$3:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -275,7 +276,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>finance.csv!$L$10:$L$14</c:f>
+              <c:f>standard!$L$10:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -303,7 +304,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>finance.csv!$M$1</c:f>
+              <c:f>standard!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -315,7 +316,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>finance.csv!$A$3:$A$7</c:f>
+              <c:f>standard!$A$3:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -338,7 +339,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>finance.csv!$Q$10:$Q$14</c:f>
+              <c:f>standard!$Q$10:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -366,7 +367,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>finance.csv!$R$1</c:f>
+              <c:f>standard!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -378,7 +379,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>finance.csv!$A$3:$A$7</c:f>
+              <c:f>standard!$A$3:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -401,7 +402,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>finance.csv!$V$10:$V$14</c:f>
+              <c:f>standard!$V$10:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -433,11 +434,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="6073416"/>
-        <c:axId val="654519256"/>
+        <c:axId val="2531368"/>
+        <c:axId val="402516552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="6073416"/>
+        <c:axId val="2531368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -470,7 +471,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="654519256"/>
+        <c:crossAx val="402516552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -478,7 +479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="654519256"/>
+        <c:axId val="402516552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,7 +509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="6073416"/>
+        <c:crossAx val="2531368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -517,6 +518,394 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>big!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Interpreted LMS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>big!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>axfinder</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brokerspread</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>brokervariance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pricespread</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>vwap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>big!$G$10:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.152804099412842</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.510833075447175</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.117965146661214</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.167394135152782</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.205370082028153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>big!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ToasterBooster</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>big!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>axfinder</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brokerspread</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>brokervariance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pricespread</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>vwap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>big!$L$10:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.209293266265903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.10050256854614</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.757840486522921</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.146133294239927</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.208245343301728</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>big!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>New Scala Gen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>big!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>axfinder</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brokerspread</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>brokervariance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pricespread</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>vwap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>big!$Q$10:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>big!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K3Optimizer -O3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>big!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>axfinder</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>brokerspread</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>brokervariance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pricespread</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>vwap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>big!$V$10:$V$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.675814458336873</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.053772977656743</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.704943236468013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.376314920195347</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.139166266682794</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="514124024"/>
+        <c:axId val="514129848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="514124024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Financial</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Queries</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="514129848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="514129848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution Time (Normalized)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="514124024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.658944881889764"/>
+          <c:y val="0.0504050954669627"/>
+          <c:w val="0.205229019769203"/>
+          <c:h val="0.299186791595185"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -549,6 +938,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1415,7 +1841,545 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V14"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0.03</v>
+      </c>
+      <c r="C3">
+        <v>1.0309999999999999</v>
+      </c>
+      <c r="D3">
+        <v>5.117</v>
+      </c>
+      <c r="E3">
+        <v>3.6039460000000001</v>
+      </c>
+      <c r="F3">
+        <v>3.411286</v>
+      </c>
+      <c r="G3">
+        <v>3.9891610000000002</v>
+      </c>
+      <c r="H3">
+        <v>31.457999999999998</v>
+      </c>
+      <c r="I3">
+        <v>2.823</v>
+      </c>
+      <c r="J3">
+        <v>3.383915</v>
+      </c>
+      <c r="K3">
+        <v>3.3214070000000002</v>
+      </c>
+      <c r="L3">
+        <v>4.1846360000000002</v>
+      </c>
+      <c r="M3">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="N3">
+        <v>1.155</v>
+      </c>
+      <c r="O3">
+        <v>3.2139709999999999</v>
+      </c>
+      <c r="P3">
+        <v>2.9227110000000001</v>
+      </c>
+      <c r="Q3">
+        <v>3.4603980000000001</v>
+      </c>
+      <c r="R3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="S3">
+        <v>1.853</v>
+      </c>
+      <c r="T3">
+        <v>5.2677449999999997</v>
+      </c>
+      <c r="U3">
+        <v>5.1803030000000003</v>
+      </c>
+      <c r="V3">
+        <v>5.7989850000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C4">
+        <v>0.221</v>
+      </c>
+      <c r="D4">
+        <v>0.626</v>
+      </c>
+      <c r="E4">
+        <v>1.7298519999999999</v>
+      </c>
+      <c r="F4">
+        <v>1.689629</v>
+      </c>
+      <c r="G4">
+        <v>2.4410530000000001</v>
+      </c>
+      <c r="H4">
+        <v>21.216000000000001</v>
+      </c>
+      <c r="I4">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="J4">
+        <v>8.1262849999999993</v>
+      </c>
+      <c r="K4">
+        <v>7.8859469999999998</v>
+      </c>
+      <c r="L4">
+        <v>8.2408819999999992</v>
+      </c>
+      <c r="M4">
+        <v>4.7E-2</v>
+      </c>
+      <c r="N4">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="O4">
+        <v>1.5030790000000001</v>
+      </c>
+      <c r="P4">
+        <v>1.4910490000000001</v>
+      </c>
+      <c r="Q4">
+        <v>1.6156999999999999</v>
+      </c>
+      <c r="R4">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="S4">
+        <v>1.196</v>
+      </c>
+      <c r="T4">
+        <v>14.485011</v>
+      </c>
+      <c r="U4">
+        <v>14.190554000000001</v>
+      </c>
+      <c r="V4">
+        <v>14.628181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="C5">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E5">
+        <v>0.25071199999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.23454700000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.29522999999999999</v>
+      </c>
+      <c r="H5">
+        <v>12.669</v>
+      </c>
+      <c r="I5">
+        <v>0.73</v>
+      </c>
+      <c r="J5">
+        <v>0.41711799999999999</v>
+      </c>
+      <c r="K5">
+        <v>0.40428700000000001</v>
+      </c>
+      <c r="L5">
+        <v>0.46420699999999998</v>
+      </c>
+      <c r="M5">
+        <v>2.7E-2</v>
+      </c>
+      <c r="N5">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="O5">
+        <v>0.25382500000000002</v>
+      </c>
+      <c r="P5">
+        <v>0.242977</v>
+      </c>
+      <c r="Q5">
+        <v>0.26407799999999998</v>
+      </c>
+      <c r="R5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="S5">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="T5">
+        <v>0.41547299999999998</v>
+      </c>
+      <c r="U5">
+        <v>0.40252900000000003</v>
+      </c>
+      <c r="V5">
+        <v>0.45023800000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="E6">
+        <v>18.208698999999999</v>
+      </c>
+      <c r="F6">
+        <v>17.935727</v>
+      </c>
+      <c r="G6">
+        <v>18.426636999999999</v>
+      </c>
+      <c r="H6">
+        <v>33.533999999999999</v>
+      </c>
+      <c r="I6">
+        <v>1.157</v>
+      </c>
+      <c r="J6">
+        <v>17.866958</v>
+      </c>
+      <c r="K6">
+        <v>17.705908999999998</v>
+      </c>
+      <c r="L6">
+        <v>18.091047</v>
+      </c>
+      <c r="M6">
+        <v>0.1</v>
+      </c>
+      <c r="N6">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="O6">
+        <v>15.595147000000001</v>
+      </c>
+      <c r="P6">
+        <v>15.363842</v>
+      </c>
+      <c r="Q6">
+        <v>15.784418000000001</v>
+      </c>
+      <c r="R6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="S6">
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="T6">
+        <v>21.383738999999998</v>
+      </c>
+      <c r="U6">
+        <v>21.160083</v>
+      </c>
+      <c r="V6">
+        <v>21.724329999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="C7">
+        <v>0.11</v>
+      </c>
+      <c r="D7">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="E7">
+        <v>3.065226</v>
+      </c>
+      <c r="F7">
+        <v>3.0412699999999999</v>
+      </c>
+      <c r="G7">
+        <v>3.1290659999999999</v>
+      </c>
+      <c r="H7">
+        <v>18.425000000000001</v>
+      </c>
+      <c r="I7">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="J7">
+        <v>3.0903779999999998</v>
+      </c>
+      <c r="K7">
+        <v>3.051069</v>
+      </c>
+      <c r="L7">
+        <v>3.13653</v>
+      </c>
+      <c r="M7">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="N7">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="O7">
+        <v>2.555625</v>
+      </c>
+      <c r="P7">
+        <v>2.5491959999999998</v>
+      </c>
+      <c r="Q7">
+        <v>2.5959379999999999</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="T7">
+        <v>13.185905</v>
+      </c>
+      <c r="U7">
+        <v>12.985325</v>
+      </c>
+      <c r="V7">
+        <v>13.340957</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="G10">
+        <f>(G3/$Q3)</f>
+        <v>1.1528040994128421</v>
+      </c>
+      <c r="L10">
+        <f>(L3/$Q3)</f>
+        <v>1.2092932662659035</v>
+      </c>
+      <c r="Q10">
+        <f>(Q3/$Q3)</f>
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <f>(V3/$Q3)</f>
+        <v>1.6758144583368733</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="G11">
+        <f>(G4/$Q4)</f>
+        <v>1.5108330754471748</v>
+      </c>
+      <c r="L11">
+        <f>(L4/$Q4)</f>
+        <v>5.1005025685461405</v>
+      </c>
+      <c r="Q11">
+        <f>(Q4/$Q4)</f>
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <f>(V4/$Q4)</f>
+        <v>9.0537729776567435</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="G12">
+        <f>(G5/$Q5)</f>
+        <v>1.1179651466612137</v>
+      </c>
+      <c r="L12">
+        <f>(L5/$Q5)</f>
+        <v>1.7578404865229214</v>
+      </c>
+      <c r="Q12">
+        <f>(Q5/$Q5)</f>
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <f>(V5/$Q5)</f>
+        <v>1.7049432364680135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="G13">
+        <f>(G6/$Q6)</f>
+        <v>1.1673941351527817</v>
+      </c>
+      <c r="L13">
+        <f>(L6/$Q6)</f>
+        <v>1.1461332942399269</v>
+      </c>
+      <c r="Q13">
+        <f>(Q6/$Q6)</f>
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <f>(V6/$Q6)</f>
+        <v>1.3763149201953468</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="G14">
+        <f>(G7/$Q7)</f>
+        <v>1.2053700820281532</v>
+      </c>
+      <c r="L14">
+        <f>(L7/$Q7)</f>
+        <v>1.2082453433017277</v>
+      </c>
+      <c r="Q14">
+        <f>(Q7/$Q7)</f>
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <f>(V7/$Q7)</f>
+        <v>5.1391662666827944</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>